<commit_message>
cleanup attempt #1 - turn list of special words into txt file
</commit_message>
<xml_diff>
--- a/data/Woolies bakery info.xlsx
+++ b/data/Woolies bakery info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nplon\Documents\Legacy\Code\Grocery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebProjects\grecy-api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C49F20D-33A1-4FE8-8412-411F36B403E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31516BD3-0808-4A6D-A4E3-C819080B1EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7683,12 +7683,12 @@
       <selection activeCell="A216" sqref="A216"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="18" max="18" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="255.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -7830,7 +7830,7 @@
         <v>2108</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -7901,7 +7901,7 @@
         <v>2109</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -7969,7 +7969,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>2111</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>2112</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -8179,7 +8179,7 @@
         <v>2113</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -8250,7 +8250,7 @@
         <v>2114</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -8315,7 +8315,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -8386,7 +8386,7 @@
         <v>2116</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -8451,7 +8451,7 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -8522,7 +8522,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -8587,7 +8587,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -8658,7 +8658,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -8729,7 +8729,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -8800,7 +8800,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -8871,7 +8871,7 @@
         <v>2123</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>2124</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -9007,7 +9007,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -9075,7 +9075,7 @@
         <v>2126</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -9146,7 +9146,7 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -9217,7 +9217,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -9288,7 +9288,7 @@
         <v>2129</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -9353,7 +9353,7 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -9421,7 +9421,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -9492,7 +9492,7 @@
         <v>2132</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -9557,7 +9557,7 @@
         <v>2133</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -9622,7 +9622,7 @@
         <v>2134</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -9693,7 +9693,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -9764,7 +9764,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -9829,7 +9829,7 @@
         <v>2137</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -9897,7 +9897,7 @@
         <v>2138</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -9968,7 +9968,7 @@
         <v>2139</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -10036,7 +10036,7 @@
         <v>2140</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -10107,7 +10107,7 @@
         <v>2141</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -10172,7 +10172,7 @@
         <v>2142</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -10237,7 +10237,7 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>59</v>
       </c>
@@ -10308,7 +10308,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -10376,7 +10376,7 @@
         <v>2144</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>61</v>
       </c>
@@ -10447,7 +10447,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>62</v>
       </c>
@@ -10515,7 +10515,7 @@
         <v>2146</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>63</v>
       </c>
@@ -10574,7 +10574,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>64</v>
       </c>
@@ -10645,7 +10645,7 @@
         <v>2147</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>65</v>
       </c>
@@ -10716,7 +10716,7 @@
         <v>2148</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -10787,7 +10787,7 @@
         <v>2149</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>67</v>
       </c>
@@ -10852,7 +10852,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>68</v>
       </c>
@@ -10920,7 +10920,7 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>69</v>
       </c>
@@ -10988,7 +10988,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -11056,7 +11056,7 @@
         <v>2152</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>71</v>
       </c>
@@ -11121,7 +11121,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>72</v>
       </c>
@@ -11189,7 +11189,7 @@
         <v>2153</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>73</v>
       </c>
@@ -11260,7 +11260,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>74</v>
       </c>
@@ -11328,7 +11328,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>75</v>
       </c>
@@ -11396,7 +11396,7 @@
         <v>2156</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -11464,7 +11464,7 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -11535,7 +11535,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>78</v>
       </c>
@@ -11603,7 +11603,7 @@
         <v>2159</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>79</v>
       </c>
@@ -11659,7 +11659,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>80</v>
       </c>
@@ -11730,7 +11730,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -11795,7 +11795,7 @@
         <v>2161</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -11866,7 +11866,7 @@
         <v>2162</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>83</v>
       </c>
@@ -11937,7 +11937,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>84</v>
       </c>
@@ -12008,7 +12008,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>85</v>
       </c>
@@ -12079,7 +12079,7 @@
         <v>2165</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>86</v>
       </c>
@@ -12147,7 +12147,7 @@
         <v>2166</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>87</v>
       </c>
@@ -12218,7 +12218,7 @@
         <v>2167</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>88</v>
       </c>
@@ -12289,7 +12289,7 @@
         <v>2168</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>89</v>
       </c>
@@ -12360,7 +12360,7 @@
         <v>2169</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>90</v>
       </c>
@@ -12431,7 +12431,7 @@
         <v>2170</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>91</v>
       </c>
@@ -12496,7 +12496,7 @@
         <v>2171</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>92</v>
       </c>
@@ -12567,7 +12567,7 @@
         <v>2172</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>93</v>
       </c>
@@ -12623,7 +12623,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>94</v>
       </c>
@@ -12694,7 +12694,7 @@
         <v>2173</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>95</v>
       </c>
@@ -12759,7 +12759,7 @@
         <v>2174</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>96</v>
       </c>
@@ -12827,7 +12827,7 @@
         <v>2175</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>97</v>
       </c>
@@ -12883,7 +12883,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>98</v>
       </c>
@@ -12954,7 +12954,7 @@
         <v>2176</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>99</v>
       </c>
@@ -13025,7 +13025,7 @@
         <v>2177</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>100</v>
       </c>
@@ -13096,7 +13096,7 @@
         <v>2178</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>101</v>
       </c>
@@ -13161,7 +13161,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>102</v>
       </c>
@@ -13232,7 +13232,7 @@
         <v>2180</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>103</v>
       </c>
@@ -13300,7 +13300,7 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>104</v>
       </c>
@@ -13371,7 +13371,7 @@
         <v>2182</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>105</v>
       </c>
@@ -13433,7 +13433,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>106</v>
       </c>
@@ -13501,7 +13501,7 @@
         <v>2184</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>107</v>
       </c>
@@ -13572,7 +13572,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>108</v>
       </c>
@@ -13640,7 +13640,7 @@
         <v>2186</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>109</v>
       </c>
@@ -13708,7 +13708,7 @@
         <v>2187</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>110</v>
       </c>
@@ -13779,7 +13779,7 @@
         <v>2188</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>111</v>
       </c>
@@ -13847,7 +13847,7 @@
         <v>2189</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>112</v>
       </c>
@@ -13915,7 +13915,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>113</v>
       </c>
@@ -13986,7 +13986,7 @@
         <v>2191</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>114</v>
       </c>
@@ -14057,7 +14057,7 @@
         <v>2192</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>115</v>
       </c>
@@ -14125,7 +14125,7 @@
         <v>2193</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>116</v>
       </c>
@@ -14193,7 +14193,7 @@
         <v>2194</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>117</v>
       </c>
@@ -14258,7 +14258,7 @@
         <v>2195</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>118</v>
       </c>
@@ -14329,7 +14329,7 @@
         <v>2196</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>119</v>
       </c>
@@ -14400,7 +14400,7 @@
         <v>2197</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>120</v>
       </c>
@@ -14465,7 +14465,7 @@
         <v>2198</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>121</v>
       </c>
@@ -14533,7 +14533,7 @@
         <v>2199</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>122</v>
       </c>
@@ -14601,7 +14601,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>123</v>
       </c>
@@ -14669,7 +14669,7 @@
         <v>2201</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>124</v>
       </c>
@@ -14734,7 +14734,7 @@
         <v>2202</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>125</v>
       </c>
@@ -14796,7 +14796,7 @@
         <v>2203</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>126</v>
       </c>
@@ -14867,7 +14867,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>127</v>
       </c>
@@ -14938,7 +14938,7 @@
         <v>2205</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>128</v>
       </c>
@@ -15006,7 +15006,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>129</v>
       </c>
@@ -15074,7 +15074,7 @@
         <v>2207</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>130</v>
       </c>
@@ -15145,7 +15145,7 @@
         <v>2208</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>86</v>
       </c>
@@ -15216,7 +15216,7 @@
         <v>2209</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>131</v>
       </c>
@@ -15287,7 +15287,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>132</v>
       </c>
@@ -15358,7 +15358,7 @@
         <v>2211</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>133</v>
       </c>
@@ -15429,7 +15429,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>134</v>
       </c>
@@ -15500,7 +15500,7 @@
         <v>2213</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>135</v>
       </c>
@@ -15568,7 +15568,7 @@
         <v>2214</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>136</v>
       </c>
@@ -15639,7 +15639,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>137</v>
       </c>
@@ -15707,7 +15707,7 @@
         <v>2216</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>138</v>
       </c>
@@ -15775,7 +15775,7 @@
         <v>2217</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>139</v>
       </c>
@@ -15843,7 +15843,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>140</v>
       </c>
@@ -15914,7 +15914,7 @@
         <v>2219</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>141</v>
       </c>
@@ -15979,7 +15979,7 @@
         <v>2220</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>142</v>
       </c>
@@ -16047,7 +16047,7 @@
         <v>2221</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>143</v>
       </c>
@@ -16112,7 +16112,7 @@
         <v>2222</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>144</v>
       </c>
@@ -16180,7 +16180,7 @@
         <v>2102</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>145</v>
       </c>
@@ -16245,7 +16245,7 @@
         <v>2223</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>146</v>
       </c>
@@ -16313,7 +16313,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>131</v>
       </c>
@@ -16384,7 +16384,7 @@
         <v>2225</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>147</v>
       </c>
@@ -16455,7 +16455,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>148</v>
       </c>
@@ -16526,7 +16526,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>149</v>
       </c>
@@ -16591,7 +16591,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>150</v>
       </c>
@@ -16659,7 +16659,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>151</v>
       </c>
@@ -16730,7 +16730,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>152</v>
       </c>
@@ -16798,7 +16798,7 @@
         <v>2231</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>153</v>
       </c>
@@ -16866,7 +16866,7 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>154</v>
       </c>
@@ -16925,7 +16925,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>155</v>
       </c>
@@ -16993,7 +16993,7 @@
         <v>2233</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>156</v>
       </c>
@@ -17064,7 +17064,7 @@
         <v>2234</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>157</v>
       </c>
@@ -17135,7 +17135,7 @@
         <v>2235</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>158</v>
       </c>
@@ -17203,7 +17203,7 @@
         <v>2236</v>
       </c>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>159</v>
       </c>
@@ -17271,7 +17271,7 @@
         <v>2237</v>
       </c>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>160</v>
       </c>
@@ -17336,7 +17336,7 @@
         <v>2238</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>161</v>
       </c>
@@ -17407,7 +17407,7 @@
         <v>2239</v>
       </c>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>162</v>
       </c>
@@ -17475,7 +17475,7 @@
         <v>2240</v>
       </c>
     </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>163</v>
       </c>
@@ -17543,7 +17543,7 @@
         <v>2241</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>164</v>
       </c>
@@ -17614,7 +17614,7 @@
         <v>2242</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>165</v>
       </c>
@@ -17679,7 +17679,7 @@
         <v>2243</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>166</v>
       </c>
@@ -17747,7 +17747,7 @@
         <v>2244</v>
       </c>
     </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>167</v>
       </c>
@@ -17815,7 +17815,7 @@
         <v>2245</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>168</v>
       </c>
@@ -17880,7 +17880,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>169</v>
       </c>
@@ -17936,7 +17936,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>170</v>
       </c>
@@ -18004,7 +18004,7 @@
         <v>2247</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>171</v>
       </c>
@@ -18075,7 +18075,7 @@
         <v>2248</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>172</v>
       </c>
@@ -18140,7 +18140,7 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>173</v>
       </c>
@@ -18208,7 +18208,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>174</v>
       </c>
@@ -18276,7 +18276,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>175</v>
       </c>
@@ -18347,7 +18347,7 @@
         <v>2252</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>176</v>
       </c>
@@ -18418,7 +18418,7 @@
         <v>2253</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>177</v>
       </c>
@@ -18489,7 +18489,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>178</v>
       </c>
@@ -18554,7 +18554,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>179</v>
       </c>
@@ -18619,7 +18619,7 @@
         <v>2256</v>
       </c>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>180</v>
       </c>
@@ -18684,7 +18684,7 @@
         <v>2257</v>
       </c>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>181</v>
       </c>
@@ -18752,7 +18752,7 @@
         <v>2258</v>
       </c>
     </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>182</v>
       </c>
@@ -18823,7 +18823,7 @@
         <v>2259</v>
       </c>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>183</v>
       </c>
@@ -18894,7 +18894,7 @@
         <v>2260</v>
       </c>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>184</v>
       </c>
@@ -18965,7 +18965,7 @@
         <v>2261</v>
       </c>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>185</v>
       </c>
@@ -19024,7 +19024,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>186</v>
       </c>
@@ -19080,7 +19080,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>187</v>
       </c>
@@ -19148,7 +19148,7 @@
         <v>2262</v>
       </c>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>188</v>
       </c>
@@ -19216,7 +19216,7 @@
         <v>2263</v>
       </c>
     </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>189</v>
       </c>
@@ -19287,7 +19287,7 @@
         <v>2264</v>
       </c>
     </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>190</v>
       </c>
@@ -19352,7 +19352,7 @@
         <v>2265</v>
       </c>
     </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>191</v>
       </c>
@@ -19423,7 +19423,7 @@
         <v>2266</v>
       </c>
     </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>192</v>
       </c>
@@ -19488,7 +19488,7 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="174" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>193</v>
       </c>
@@ -19556,7 +19556,7 @@
         <v>2268</v>
       </c>
     </row>
-    <row r="175" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>194</v>
       </c>
@@ -19612,7 +19612,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="176" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>195</v>
       </c>
@@ -19677,7 +19677,7 @@
         <v>2269</v>
       </c>
     </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>196</v>
       </c>
@@ -19745,7 +19745,7 @@
         <v>2270</v>
       </c>
     </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>197</v>
       </c>
@@ -19816,7 +19816,7 @@
         <v>2271</v>
       </c>
     </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>198</v>
       </c>
@@ -19881,7 +19881,7 @@
         <v>2272</v>
       </c>
     </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>199</v>
       </c>
@@ -19949,7 +19949,7 @@
         <v>2273</v>
       </c>
     </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>200</v>
       </c>
@@ -20020,7 +20020,7 @@
         <v>2274</v>
       </c>
     </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>201</v>
       </c>
@@ -20079,7 +20079,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>202</v>
       </c>
@@ -20150,7 +20150,7 @@
         <v>2275</v>
       </c>
     </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>203</v>
       </c>
@@ -20218,7 +20218,7 @@
         <v>2276</v>
       </c>
     </row>
-    <row r="185" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>204</v>
       </c>
@@ -20286,7 +20286,7 @@
         <v>2277</v>
       </c>
     </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>205</v>
       </c>
@@ -20357,7 +20357,7 @@
         <v>2278</v>
       </c>
     </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>206</v>
       </c>
@@ -20428,7 +20428,7 @@
         <v>2279</v>
       </c>
     </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>207</v>
       </c>
@@ -20493,7 +20493,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>208</v>
       </c>
@@ -20558,7 +20558,7 @@
         <v>2281</v>
       </c>
     </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>209</v>
       </c>
@@ -20626,7 +20626,7 @@
         <v>2282</v>
       </c>
     </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>210</v>
       </c>
@@ -20697,7 +20697,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="192" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>211</v>
       </c>
@@ -20765,7 +20765,7 @@
         <v>2284</v>
       </c>
     </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>212</v>
       </c>
@@ -20836,7 +20836,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="194" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>213</v>
       </c>
@@ -20904,7 +20904,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>214</v>
       </c>
@@ -20975,7 +20975,7 @@
         <v>2287</v>
       </c>
     </row>
-    <row r="196" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>215</v>
       </c>
@@ -21046,7 +21046,7 @@
         <v>2288</v>
       </c>
     </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>216</v>
       </c>
@@ -21111,7 +21111,7 @@
         <v>2289</v>
       </c>
     </row>
-    <row r="198" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>217</v>
       </c>
@@ -21176,7 +21176,7 @@
         <v>2290</v>
       </c>
     </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>218</v>
       </c>
@@ -21247,7 +21247,7 @@
         <v>2291</v>
       </c>
     </row>
-    <row r="200" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>219</v>
       </c>
@@ -21315,7 +21315,7 @@
         <v>2292</v>
       </c>
     </row>
-    <row r="201" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>220</v>
       </c>
@@ -21386,7 +21386,7 @@
         <v>2293</v>
       </c>
     </row>
-    <row r="202" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>221</v>
       </c>
@@ -21454,7 +21454,7 @@
         <v>2294</v>
       </c>
     </row>
-    <row r="203" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>222</v>
       </c>
@@ -21522,7 +21522,7 @@
         <v>2295</v>
       </c>
     </row>
-    <row r="204" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>223</v>
       </c>
@@ -21590,7 +21590,7 @@
         <v>2296</v>
       </c>
     </row>
-    <row r="205" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>224</v>
       </c>
@@ -21646,7 +21646,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="206" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>225</v>
       </c>
@@ -21717,7 +21717,7 @@
         <v>2297</v>
       </c>
     </row>
-    <row r="207" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>226</v>
       </c>
@@ -21773,7 +21773,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="208" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>227</v>
       </c>
@@ -21838,7 +21838,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="209" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>228</v>
       </c>
@@ -21906,7 +21906,7 @@
         <v>2299</v>
       </c>
     </row>
-    <row r="210" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>229</v>
       </c>
@@ -21971,7 +21971,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="211" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>230</v>
       </c>
@@ -22039,7 +22039,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="212" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>231</v>
       </c>
@@ -22110,7 +22110,7 @@
         <v>2302</v>
       </c>
     </row>
-    <row r="213" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>232</v>
       </c>
@@ -22181,7 +22181,7 @@
         <v>2303</v>
       </c>
     </row>
-    <row r="214" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>233</v>
       </c>
@@ -22252,7 +22252,7 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="215" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>234</v>
       </c>
@@ -22323,7 +22323,7 @@
         <v>2305</v>
       </c>
     </row>
-    <row r="216" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>235</v>
       </c>
@@ -22379,7 +22379,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="217" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>236</v>
       </c>
@@ -22450,7 +22450,7 @@
         <v>2306</v>
       </c>
     </row>
-    <row r="218" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>237</v>
       </c>
@@ -22521,7 +22521,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="219" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>238</v>
       </c>
@@ -22586,7 +22586,7 @@
         <v>2308</v>
       </c>
     </row>
-    <row r="220" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>239</v>
       </c>
@@ -22654,7 +22654,7 @@
         <v>2309</v>
       </c>
     </row>
-    <row r="221" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>240</v>
       </c>
@@ -22725,7 +22725,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="222" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>241</v>
       </c>
@@ -22796,7 +22796,7 @@
         <v>2311</v>
       </c>
     </row>
-    <row r="223" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>242</v>
       </c>
@@ -22861,7 +22861,7 @@
         <v>2312</v>
       </c>
     </row>
-    <row r="224" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>243</v>
       </c>
@@ -22926,7 +22926,7 @@
         <v>2313</v>
       </c>
     </row>
-    <row r="225" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>244</v>
       </c>
@@ -22997,7 +22997,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="226" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>245</v>
       </c>
@@ -23068,7 +23068,7 @@
         <v>2315</v>
       </c>
     </row>
-    <row r="227" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>246</v>
       </c>
@@ -23139,7 +23139,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="228" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>247</v>
       </c>
@@ -23207,7 +23207,7 @@
         <v>2317</v>
       </c>
     </row>
-    <row r="229" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>248</v>
       </c>
@@ -23278,7 +23278,7 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="230" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>249</v>
       </c>
@@ -23340,7 +23340,7 @@
         <v>2319</v>
       </c>
     </row>
-    <row r="231" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>250</v>
       </c>
@@ -23411,7 +23411,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="232" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>251</v>
       </c>
@@ -23476,7 +23476,7 @@
         <v>2321</v>
       </c>
     </row>
-    <row r="233" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>252</v>
       </c>
@@ -23547,7 +23547,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="234" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>253</v>
       </c>
@@ -23618,7 +23618,7 @@
         <v>2323</v>
       </c>
     </row>
-    <row r="235" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>254</v>
       </c>
@@ -23683,7 +23683,7 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="236" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>255</v>
       </c>
@@ -23751,7 +23751,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="237" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>256</v>
       </c>
@@ -23816,7 +23816,7 @@
         <v>2326</v>
       </c>
     </row>
-    <row r="238" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>257</v>
       </c>
@@ -23884,7 +23884,7 @@
         <v>2327</v>
       </c>
     </row>
-    <row r="239" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>258</v>
       </c>
@@ -23952,7 +23952,7 @@
         <v>2328</v>
       </c>
     </row>
-    <row r="240" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>259</v>
       </c>
@@ -24020,7 +24020,7 @@
         <v>2329</v>
       </c>
     </row>
-    <row r="241" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>260</v>
       </c>
@@ -24091,7 +24091,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="242" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>261</v>
       </c>
@@ -24159,7 +24159,7 @@
         <v>2331</v>
       </c>
     </row>
-    <row r="243" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>262</v>
       </c>
@@ -24230,7 +24230,7 @@
         <v>2332</v>
       </c>
     </row>
-    <row r="244" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>263</v>
       </c>
@@ -24298,7 +24298,7 @@
         <v>2333</v>
       </c>
     </row>
-    <row r="245" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>264</v>
       </c>
@@ -24366,7 +24366,7 @@
         <v>2334</v>
       </c>
     </row>
-    <row r="246" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>265</v>
       </c>
@@ -24431,7 +24431,7 @@
         <v>2335</v>
       </c>
     </row>
-    <row r="247" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>266</v>
       </c>
@@ -24502,7 +24502,7 @@
         <v>2336</v>
       </c>
     </row>
-    <row r="248" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>267</v>
       </c>
@@ -24570,7 +24570,7 @@
         <v>2337</v>
       </c>
     </row>
-    <row r="249" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>268</v>
       </c>
@@ -24641,7 +24641,7 @@
         <v>2338</v>
       </c>
     </row>
-    <row r="250" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>269</v>
       </c>
@@ -24697,7 +24697,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="251" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>270</v>
       </c>
@@ -24762,7 +24762,7 @@
         <v>2339</v>
       </c>
     </row>
-    <row r="252" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>271</v>
       </c>
@@ -24827,7 +24827,7 @@
         <v>2340</v>
       </c>
     </row>
-    <row r="253" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>272</v>
       </c>
@@ -24895,7 +24895,7 @@
         <v>2341</v>
       </c>
     </row>
-    <row r="254" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>273</v>
       </c>
@@ -24951,7 +24951,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="255" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>274</v>
       </c>
@@ -25016,7 +25016,7 @@
         <v>2342</v>
       </c>
     </row>
-    <row r="256" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>275</v>
       </c>
@@ -25087,7 +25087,7 @@
         <v>2343</v>
       </c>
     </row>
-    <row r="257" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>276</v>
       </c>
@@ -25152,7 +25152,7 @@
         <v>2344</v>
       </c>
     </row>
-    <row r="258" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>277</v>
       </c>
@@ -25220,7 +25220,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="259" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>278</v>
       </c>
@@ -25291,7 +25291,7 @@
         <v>2346</v>
       </c>
     </row>
-    <row r="260" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>279</v>
       </c>
@@ -25362,7 +25362,7 @@
         <v>2347</v>
       </c>
     </row>
-    <row r="261" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>280</v>
       </c>
@@ -25433,7 +25433,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="262" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>281</v>
       </c>
@@ -25495,7 +25495,7 @@
         <v>2349</v>
       </c>
     </row>
-    <row r="263" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>282</v>
       </c>
@@ -25560,7 +25560,7 @@
         <v>2102</v>
       </c>
     </row>
-    <row r="264" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>283</v>
       </c>
@@ -25625,7 +25625,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="265" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>284</v>
       </c>
@@ -25693,7 +25693,7 @@
         <v>2351</v>
       </c>
     </row>
-    <row r="266" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>285</v>
       </c>
@@ -25761,7 +25761,7 @@
         <v>2352</v>
       </c>
     </row>
-    <row r="267" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>286</v>
       </c>
@@ -25832,7 +25832,7 @@
         <v>2353</v>
       </c>
     </row>
-    <row r="268" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>287</v>
       </c>
@@ -25903,7 +25903,7 @@
         <v>2354</v>
       </c>
     </row>
-    <row r="269" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>288</v>
       </c>
@@ -25974,7 +25974,7 @@
         <v>2355</v>
       </c>
     </row>
-    <row r="270" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>289</v>
       </c>
@@ -26039,7 +26039,7 @@
         <v>2356</v>
       </c>
     </row>
-    <row r="271" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>290</v>
       </c>
@@ -26110,7 +26110,7 @@
         <v>2357</v>
       </c>
     </row>
-    <row r="272" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>291</v>
       </c>
@@ -26181,7 +26181,7 @@
         <v>2358</v>
       </c>
     </row>
-    <row r="273" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>292</v>
       </c>
@@ -26246,7 +26246,7 @@
         <v>2102</v>
       </c>
     </row>
-    <row r="274" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>293</v>
       </c>
@@ -26314,7 +26314,7 @@
         <v>2359</v>
       </c>
     </row>
-    <row r="275" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>294</v>
       </c>
@@ -26379,7 +26379,7 @@
         <v>2360</v>
       </c>
     </row>
-    <row r="276" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>295</v>
       </c>
@@ -26447,7 +26447,7 @@
         <v>2361</v>
       </c>
     </row>
-    <row r="277" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>296</v>
       </c>
@@ -26512,7 +26512,7 @@
         <v>2362</v>
       </c>
     </row>
-    <row r="278" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>297</v>
       </c>
@@ -26580,7 +26580,7 @@
         <v>2363</v>
       </c>
     </row>
-    <row r="279" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>298</v>
       </c>
@@ -26648,7 +26648,7 @@
         <v>2364</v>
       </c>
     </row>
-    <row r="280" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>299</v>
       </c>
@@ -26719,7 +26719,7 @@
         <v>2365</v>
       </c>
     </row>
-    <row r="281" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>300</v>
       </c>
@@ -26787,7 +26787,7 @@
         <v>2102</v>
       </c>
     </row>
-    <row r="282" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>301</v>
       </c>
@@ -26849,7 +26849,7 @@
         <v>2366</v>
       </c>
     </row>
-    <row r="283" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>302</v>
       </c>
@@ -26905,7 +26905,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="284" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>303</v>
       </c>
@@ -26961,7 +26961,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="285" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>304</v>
       </c>
@@ -27032,7 +27032,7 @@
         <v>2367</v>
       </c>
     </row>
-    <row r="286" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>305</v>
       </c>
@@ -27100,7 +27100,7 @@
         <v>2368</v>
       </c>
     </row>
-    <row r="287" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>306</v>
       </c>
@@ -27165,7 +27165,7 @@
         <v>2369</v>
       </c>
     </row>
-    <row r="288" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>307</v>
       </c>
@@ -27236,7 +27236,7 @@
         <v>2370</v>
       </c>
     </row>
-    <row r="289" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>308</v>
       </c>
@@ -27301,7 +27301,7 @@
         <v>2371</v>
       </c>
     </row>
-    <row r="290" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>309</v>
       </c>
@@ -27357,7 +27357,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="291" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>310</v>
       </c>
@@ -27416,7 +27416,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="292" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>311</v>
       </c>
@@ -27475,7 +27475,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="293" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>312</v>
       </c>
@@ -27543,7 +27543,7 @@
         <v>2372</v>
       </c>
     </row>
-    <row r="294" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>313</v>
       </c>
@@ -27608,7 +27608,7 @@
         <v>2373</v>
       </c>
     </row>
-    <row r="295" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>314</v>
       </c>
@@ -27679,7 +27679,7 @@
         <v>2374</v>
       </c>
     </row>
-    <row r="296" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>315</v>
       </c>
@@ -27750,7 +27750,7 @@
         <v>2375</v>
       </c>
     </row>
-    <row r="297" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>316</v>
       </c>
@@ -27818,7 +27818,7 @@
         <v>2376</v>
       </c>
     </row>
-    <row r="298" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>317</v>
       </c>
@@ -27886,7 +27886,7 @@
         <v>2377</v>
       </c>
     </row>
-    <row r="299" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>318</v>
       </c>
@@ -27942,7 +27942,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="300" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>318</v>
       </c>
@@ -27998,7 +27998,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="301" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>319</v>
       </c>
@@ -28069,7 +28069,7 @@
         <v>2378</v>
       </c>
     </row>
-    <row r="302" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>320</v>
       </c>
@@ -28134,7 +28134,7 @@
         <v>2379</v>
       </c>
     </row>
-    <row r="303" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>321</v>
       </c>
@@ -28205,7 +28205,7 @@
         <v>2380</v>
       </c>
     </row>
-    <row r="304" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>322</v>
       </c>
@@ -28261,7 +28261,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="305" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>323</v>
       </c>
@@ -28332,7 +28332,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="306" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>324</v>
       </c>
@@ -28397,7 +28397,7 @@
         <v>2382</v>
       </c>
     </row>
-    <row r="307" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>325</v>
       </c>
@@ -28453,7 +28453,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="308" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>326</v>
       </c>
@@ -28518,7 +28518,7 @@
         <v>2383</v>
       </c>
     </row>
-    <row r="309" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>327</v>
       </c>
@@ -28589,7 +28589,7 @@
         <v>2384</v>
       </c>
     </row>
-    <row r="310" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>328</v>
       </c>
@@ -28657,7 +28657,7 @@
         <v>2385</v>
       </c>
     </row>
-    <row r="311" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>329</v>
       </c>
@@ -28713,7 +28713,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="312" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>330</v>
       </c>
@@ -28769,7 +28769,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="313" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>331</v>
       </c>
@@ -28834,7 +28834,7 @@
         <v>2386</v>
       </c>
     </row>
-    <row r="314" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>332</v>
       </c>
@@ -28899,7 +28899,7 @@
         <v>2387</v>
       </c>
     </row>
-    <row r="315" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>333</v>
       </c>
@@ -28964,7 +28964,7 @@
         <v>2388</v>
       </c>
     </row>
-    <row r="316" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>334</v>
       </c>
@@ -29035,7 +29035,7 @@
         <v>2389</v>
       </c>
     </row>
-    <row r="317" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>335</v>
       </c>
@@ -29106,7 +29106,7 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="318" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>336</v>
       </c>
@@ -29174,7 +29174,7 @@
         <v>2391</v>
       </c>
     </row>
-    <row r="319" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>337</v>
       </c>
@@ -29242,7 +29242,7 @@
         <v>2392</v>
       </c>
     </row>
-    <row r="320" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>338</v>
       </c>
@@ -29310,7 +29310,7 @@
         <v>2393</v>
       </c>
     </row>
-    <row r="321" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>339</v>
       </c>
@@ -29366,7 +29366,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="322" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>340</v>
       </c>
@@ -29431,7 +29431,7 @@
         <v>2394</v>
       </c>
     </row>
-    <row r="323" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>341</v>
       </c>
@@ -29487,7 +29487,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="324" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>342</v>
       </c>
@@ -29552,7 +29552,7 @@
         <v>2395</v>
       </c>
     </row>
-    <row r="325" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>343</v>
       </c>
@@ -29623,7 +29623,7 @@
         <v>2396</v>
       </c>
     </row>
-    <row r="326" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>344</v>
       </c>
@@ -29688,7 +29688,7 @@
         <v>2397</v>
       </c>
     </row>
-    <row r="327" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>345</v>
       </c>
@@ -29756,7 +29756,7 @@
         <v>2398</v>
       </c>
     </row>
-    <row r="328" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>346</v>
       </c>
@@ -29821,7 +29821,7 @@
         <v>2399</v>
       </c>
     </row>
-    <row r="329" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>347</v>
       </c>
@@ -29883,7 +29883,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="330" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>348</v>
       </c>
@@ -29948,7 +29948,7 @@
         <v>2401</v>
       </c>
     </row>
-    <row r="331" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>349</v>
       </c>
@@ -30013,7 +30013,7 @@
         <v>2402</v>
       </c>
     </row>
-    <row r="332" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>350</v>
       </c>

</xml_diff>